<commit_message>
fixed for school admin
</commit_message>
<xml_diff>
--- a/cypress/fixtures/2023-001_FORMAT_PR_TEMPLATE_2023.xlsx
+++ b/cypress/fixtures/2023-001_FORMAT_PR_TEMPLATE_2023.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USTP\Downloads\POINTERSBIT FILES\Cypress Project\TESTING AUTOMATION CYPRESS\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USTP\Downloads\POINTERSBIT FILES\Cypress Project\TESTING-AUTOMATION-CYPRESS\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -504,17 +504,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -523,8 +512,19 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -768,64 +768,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
     </row>
     <row r="3" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
     </row>
     <row r="4" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I4" s="2"/>
@@ -833,55 +833,55 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="M5" s="28" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="M5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
     </row>
     <row r="6" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="M6" s="24" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="M6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
       <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="M7" s="22" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="M7" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
     </row>
     <row r="8" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -889,11 +889,11 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="M8" s="24" t="s">
+      <c r="M8" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
       <c r="P8" s="20"/>
     </row>
     <row r="9" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
@@ -979,7 +979,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>28</v>
@@ -1027,7 +1027,7 @@
         <v>36</v>
       </c>
       <c r="E14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>39</v>
@@ -1075,7 +1075,7 @@
         <v>37</v>
       </c>
       <c r="E15" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>40</v>
@@ -1123,7 +1123,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>41</v>
@@ -21592,16 +21592,16 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="uyZ7okvKkXkA5HYj7tU4k9lAaKyj0xdaw5w5Tz4OioGVsLIHB57KlBrxVRdNWsVNXVKT9OXkZ+8zGP+YG966AA==" saltValue="b4q8rIZAhLIpkaHQgA3WTA==" spinCount="100000" sheet="1" objects="1"/>
   <mergeCells count="10">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="M8:O8"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="M5:P5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="M8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>